<commit_message>
sort banks by name
</commit_message>
<xml_diff>
--- a/packages/storybook/stories/data/normal.xlsx
+++ b/packages/storybook/stories/data/normal.xlsx
@@ -435,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="str">
-        <v>i65WKlGyMtBRKlSyqlZSKU4tAdF5ibmpSlZKzpklmQrOGanJ2Zl56Uo6SiWVBWBhD1dnb08/d6BIcn5OfhFQSDkpzcTY0Bgokleam5QKEgKyyzKLM5NygFpKikpTdZSK8ktLQAaB5bJTKyGM4vyiEv+iFJAeXcPa2lodsIsMTU3NLUzMLExMTQ3Noa5DUglzqgFQQywA</v>
+        <v>fY7LCsIwEEV/RUaXFZqmSZNui6gI+gHiwmrU0Ec0TYVS+u8mVaEidDWXM3OGu2/BQOx78IC4hVkljJvlsRAQQyKNnCQ3ccpkeQUPTHPv8WqRbNbbpSUnlStt0TS9hBhhS8q6SIVDNj9lJdPcKkbXwgOtauMe9btMNO9QKW12+uycOeq6zusbIUIiFlIWEoKiT7vB5beqPxQ4jTgjlAcjAvoVmI8xo3hECP4EjkJGx4XDCw==</v>
       </c>
       <c r="D2" t="str">
         <v>a372cda0d53a2f9b0f4c46d0cd3136748</v>
@@ -465,7 +465,7 @@
         <v/>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="str">
-        <v>i65WKlGyMtBRKlSyqlZSKU4tAdF5ibmpSlZKzpklmQrBiWWZeenFSjpKJZUFINFgxzBPP/dgoEByfk5+EVBEOTk51cgkDSiSV5qblAoSMjI2MQXyyzKLM5NygLpKikpTdZSK8ktLgIYB5YFy2amVEEZxflGJf1EKSJ+uYW1trQ7YTYampuYWJmYWJqamhuZQ9yGphDkWpCEWAA==</v>
+        <v>lY49D4IwEIb/ijkdMaHQlpbNOBgXHUhcjANgNY18aCkkhPDfPfxIZCFxurvn7rm8xw4shK4DDwg7WFTKDrWIcwUhrLXVsyhudHGtwAHb3gcarQ7b3SZCkJZZaZDM01R59IKkqPNEDcjzKcO50ZVOMrSsqZUDpqwtPsM97m6qfTdVaezenAdvSfq+d16ZCGOBoFxQxkjwyfdz+Q07EiQPpGBcehOCOxaE6/uC+38JklDBpyOdng==</v>
       </c>
       <c r="D3" t="str">
         <v>a372cda0d53a2f9b0f4c46d0cd3136748</v>
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="str">
-        <v>TY7BCoJAEIZfJaaOG6S5ruwttEOnQLpFh9Q1lnS31jEQ2XdvtIJOM/P988N3HgFBbhg8QY6w6hRO01xbBRJSjXqROlVpBAY4PGaY77PDKd3lGbHSNtYRXNai3IaCiOnbQk0o5hGdL93poqEeul4xcLZHbW4UU3ZXw2fprMOjq6baOvDes1kq4FwkUZxEnAfiK/j3+bMNqXB5Aw==</v>
+        <v>jY5NC4JAEIb/SkwdDVzdL72FdugUSLfokLrFkrq1roGI/73VCoQoOs3M884D774DA6HrwA3CDha1MMOsjqWAECJp5CzSIpcGHDDtdYTJOt7solUSW5apQmkL5yeW+R6zpGrKVAyIEmzPu6xlWljP6EY4oFVjZHW2sc0uon0utdJmq/NBW6K+752xFCKEcUw5JgSxV8HJ57utNxUCygJOaOD9L3DX9zn1fwjoQwgQ5vS74Frh8AA=</v>
       </c>
       <c r="D4" t="str">
         <v>a372cda0d53a2f9b0f4c46d0cd3136748</v>
@@ -547,7 +547,7 @@
         <v/>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -641,7 +641,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -783,9 +783,56 @@
         <v/>
       </c>
     </row>
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
+        <v>a3918c067d67964dd150fcfec19e6b4da</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <v>bVTbkqJIEP0Vg9i3NmxEcMWJfkBQKAdoxUbs2tkHqKqGUi6OgFwm+t+30DZGdzcqMiozK+vkycPlr19cwU35PveTm/7i/shJ0e2pnxBuyg3zorfJyhMivZmfHrg+V5GA5auqGrCz/HKUpTFNyQBlCTv3MT6RPGc1Ai/1vEFvST4+yCnP0h/ppqQF6Ym8yNysLKLejKS43wN2TxyP+eGP1N0oDCLNCtIBMJeiLL161ybctDiVpM99UMzS/J9DoVuT7vwUsowGOvejZm5UFMd8+vzMIkwHmIY0zVn7juYzSk6dDbrKPlfm5PQ1L4uOfp5X2anD5z4/P/sXeYaSJI8nvMQzE76kunK7ScZhv/CnNPFD8pyfw6c6ib9VFBfRy3D8LSI0jIrOC/ycjMX+SpPFwKtCnGwbJMTnYM9TayNWYD95UqkSAlWZANdZrYcOdOduiEYwBYvZdn2ol+tGoeZmct62tmY28nw7X4fuEBpAm5cWyzuuSIG6zLDhVK90csYjPDJT1JqJ3MBGNlCyqHw93qNGftse0Jn1rU3ecR1VbnGCamsjHbC+pqsw63iEK8MWYDNjfOsStTz1DYdHWnY2GS5upJHVSGeUMJy9UllXDAr0KPY9nGGNzfWmVMsNCLEQM9xQBvs5q3MpMOAR7rAajEJ52SqhpSq1TTtDNw1CoNUH6MH2xuUr12IjzuFmxpPdLF5tljzcRbwp2C1qwO+7VyuREEVQl0fAyL/f5S+G9a2I1WHr64tDMEJjoM0qoioVMsLQerv4e0tTqlftX3cN/j6emCObJ14d3/GcmIITw9S6n6WBns0DHR4DvZIBtcRXLWQ6dJoobD9c9wft3lkeH6HhZKsNYNqAp5UqX3Due13mUO400u38fWe3TJvbbPReF5jEecDwgQCTy6Lgbp5ZEggSb3owCrw4J288RcKiRM2whbvl8X9rd/aRJC7j75ZW+98F7p+f4cTEWBfvnrT3dblhHAvfcw6B7j5y1GWWl6IgZbXJooVefQy6HokdB6nTvHvVQz1h87yqD9wkppl41/vh3bC2tvr72VTni4aa+P0Wd9/cRWPl5aX7E/z9Dw==</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1st Source Bank</v>
+      </c>
+      <c r="E4" t="str">
+        <v>www.1stsourceonline.com</v>
+      </c>
+      <c r="F4" t="str" xml:space="preserve">
+        <v xml:space="preserve">205 W. Jefferson
+Suite 404
+South Bend, IN 46601
+USA</v>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v>data:image/svg+xml;width=16;height=16;base64,PD94bWwgdmVyc2lvbj0iMS4wIj8+CiAgICA8IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPgogICAgPHN2ZyB4bWxucz0iaHR0cDovL3d3dy53My5vcmcvMjAwMC9zdmciIGhlaWdodD0iMTAwJSIgd2lkdGg9IjEwMCUiIHZpZXdCb3g9JzAgMCAxNiAxNic+CiAgICAgIDxkZWZzPgogICAgICAgIDxzdHlsZSB0eXBlPSJ0ZXh0L2NzcyI+CiAgICAgICAgICAuc2hhZG93IHsKICAgICAgICAgICAgdGV4dC1zaGFkb3c6IDBweCAwcHggMTBweCAjMDAwODsKICAgICAgICAgIH0KICAgICAgICA8L3N0eWxlPgogICAgICA8L2RlZnM+CiAgICAgIDxyZWN0IGZpbGw9IiM4ODgiIHg9IjAiIHk9IjAiIGhlaWdodD0iMTYiIHdpZHRoPSIxNiI+PC9yZWN0PgogICAgICA8dGV4dAogICAgICAgIGNsYXNzPSJzaGFkb3ciCiAgICAgICAgZmlsbD0iI2ZmZmZmZiIKICAgICAgICBmb250LWZhbWlseT0ic2Fucy1zZXJpZiIKICAgICAgICBmb250LXNpemU9IjUuMzMzMzMzMzMzMzMzMzMzIgogICAgICAgIHRleHQtYW5jaG9yPSJtaWRkbGUiCiAgICAgICAgZG9taW5hbnQtYmFzZWxpbmU9ImNlbnRyYWwiCiAgICAgICAgeD0iOCIKICAgICAgICB5PSI4IgogICAgICA+CiAgICAgICAgMVNCCiAgICAgIDwvdGV4dD4KICAgIDwvc3ZnPgogIA==</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="str">
+        <v>071212128</v>
+      </c>
+      <c r="K4" t="str">
+        <v>DI</v>
+      </c>
+      <c r="L4" t="str">
+        <v>https://ofxdi.diginsite.com/cmr/cmr.ofx</v>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -909,7 +956,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -922,9 +969,17 @@
         <v>value</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>sidebarWidth</v>
+      </c>
+      <c r="B2" t="str">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>